<commit_message>
Agregar pass al codigo
</commit_message>
<xml_diff>
--- a/AdministradorTI/archivos/plantillas_excel/PLANTILLA-USUARIOS-NUEVOS.xlsx
+++ b/AdministradorTI/archivos/plantillas_excel/PLANTILLA-USUARIOS-NUEVOS.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -22,9 +22,116 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
   <si>
     <t xml:space="preserve">CRAC INCASUR S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORMATO:
+FR-TI-003-2010
+Versión 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORMATO DE ENTREGA USUARIO Y CLAVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATOS DEL USUARIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombres Completos:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARPIO ARAGON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de Ingreso:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cargo:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EJECUTIVO COMERCIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLES DE RED INTERNA, INTERNET Y CORREO ELECTRÓNICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de Activación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceso a Internet:   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEACUERDO AL PROC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C. Electrónico:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcarpio@cajaincasur.com.pe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario de Sistema:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario de Sentinel:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71504321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario Windows:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario Reloj Control:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.1.225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario de Correo:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCARPIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario SBS:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcarpioa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario Impresora:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ip asignada:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFORMACIÓN DE CLAVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*  El área de TI desconoce cualquier clave que usted como usuario haya creado ademas las clave que se indica en el presente documento es de uso estricto del usuario y sera cambiada, la primera vez que el usuario ingrese al sistema de forma obligatoria, siendo el usuario el responsable de los procesos que se realicen en el sistema con el usuario asignado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la primera vez que el usuario ingrese al sistema de forma obligatoria, siendo el usuario el respon-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sable de los procesos que se realicen en el sistema con el usuario asignado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AREA DE TI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Declaro haber recibido el documento de creacion de cuenta con los usuario y claves correspondientes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario</t>
   </si>
   <si>
     <t xml:space="preserve">FORMATO:
@@ -32,154 +139,55 @@
 Versión 1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">FORMATO DE ENTREGA USUARIO Y CLAVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATOS DEL USUARIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombres Completos:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CARPIO ARAGON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de Ingreso:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cargo:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EJECUTIVO COMERCIAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLES DE RED INTERNA, INTERNET Y CORREO ELECTRÓNICO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de Activación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceso a Internet:   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEACUERDO AL PROC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Electrónico:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcarpio@cajaincasur.com.pe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario de Sistema:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario de Sentinel:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71504321</t>
+    <t xml:space="preserve">Apellidos:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAMANI LOPEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombres:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YESSICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROMOTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ymamani@cajaincasur.com.pe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0558</t>
   </si>
   <si>
     <t xml:space="preserve">Clave de Usuario del Sistema:</t>
   </si>
   <si>
-    <t xml:space="preserve">********</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ip asignada:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192.168.1.225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario de Correo:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCARPIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario SBS:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcarpioa</t>
+    <t xml:space="preserve">*****</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clave de usuario de Red:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">****</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YMAMANI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ymamanil</t>
   </si>
   <si>
     <t xml:space="preserve">Clave del Correo:</t>
   </si>
   <si>
-    <t xml:space="preserve">******</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clave del usuario SBS:</t>
   </si>
   <si>
-    <t xml:space="preserve">Usuario Impresora:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INFORMACIÓN DE CLAVE</t>
+    <t xml:space="preserve">0084</t>
   </si>
   <si>
     <t xml:space="preserve">*  La clave que se indica en el presente documento es de uso extricto del usuario y sera cambiada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">la primera vez que el usuario ingrese al sistema de forma obligatoria, siendo el usuario el respon-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sable de los procesos que se realicen en el sistema con el usuario asignado.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AREA DE TI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Declaro haber recibido el documento de creacion de cuenta con los usuario y claves correspondientes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apellidos:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAMANI LOPEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombres:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YESSICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROMOTOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ymamani@cajaincasur.com.pe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*****</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clave de usuario de Red:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">****</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YMAMANI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ymamanil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0084</t>
   </si>
   <si>
     <t xml:space="preserve">PECHORTINTA HUANCA</t>
@@ -222,6 +230,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -243,12 +252,14 @@
       <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -256,6 +267,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -263,6 +275,7 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -270,18 +283,21 @@
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -289,12 +305,14 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -302,6 +320,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -311,6 +330,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -319,12 +339,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -332,6 +354,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -339,12 +362,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -352,6 +377,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -359,12 +385,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -372,6 +400,7 @@
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -379,6 +408,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -431,7 +461,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -490,6 +520,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
       <top/>
@@ -596,68 +633,68 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -665,11 +702,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -677,43 +714,47 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -920,10 +961,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R11" activeCellId="0" sqref="R11"/>
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.4296875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -973,7 +1014,7 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -999,7 +1040,7 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1026,7 +1067,7 @@
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -1055,7 +1096,7 @@
       <c r="V5" s="8"/>
       <c r="W5" s="9"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -1066,7 +1107,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="10" t="n">
         <f aca="true">TODAY()</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -1087,7 +1128,7 @@
       <c r="V6" s="12"/>
       <c r="W6" s="9"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1120,7 +1161,7 @@
       </c>
       <c r="F8" s="10" t="n">
         <f aca="true">TODAY()</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1185,14 +1226,12 @@
       <c r="A11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
@@ -1200,7 +1239,7 @@
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S11" s="18"/>
       <c r="T11" s="18"/>
@@ -1209,16 +1248,16 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="19" t="s">
         <v>23</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>24</v>
       </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="L12" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
@@ -1226,7 +1265,7 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
@@ -1235,97 +1274,163 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
-      <c r="R13" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="S13" s="20"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="20"/>
+      <c r="R13" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="15"/>
       <c r="W13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="22"/>
+      <c r="W15" s="22"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="22"/>
+      <c r="W16" s="22"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="W16" s="9"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="W17" s="9"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="W18" s="9"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13"/>
@@ -1334,7 +1439,7 @@
     <row r="20" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="13"/>
       <c r="I20" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1345,83 +1450,83 @@
     </row>
     <row r="21" customFormat="false" ht="16.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
       <c r="W21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
       <c r="W22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
       <c r="W23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="25"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="26"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="25"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
@@ -1431,7 +1536,7 @@
       <c r="A27" s="5"/>
       <c r="W27" s="9"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
         <v>3</v>
       </c>
@@ -1458,7 +1563,7 @@
       <c r="V28" s="7"/>
       <c r="W28" s="7"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1593,7 @@
       <c r="V29" s="8"/>
       <c r="W29" s="9"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
         <v>6</v>
       </c>
@@ -1499,7 +1604,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="10" t="n">
         <f aca="false">G6</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
@@ -1507,18 +1612,18 @@
       <c r="L30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="N30" s="26" t="str">
+      <c r="N30" s="27" t="str">
         <f aca="false">N6</f>
         <v>EJECUTIVO COMERCIAL</v>
       </c>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="26"/>
-      <c r="T30" s="26"/>
-      <c r="U30" s="26"/>
-      <c r="V30" s="26"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="27"/>
+      <c r="V30" s="27"/>
       <c r="W30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,7 +1636,7 @@
       </c>
       <c r="F32" s="10" t="n">
         <f aca="false">F8</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -1539,45 +1644,45 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
-      <c r="H33" s="27"/>
-      <c r="S33" s="27"/>
+      <c r="H33" s="28"/>
+      <c r="S33" s="28"/>
       <c r="W33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="28"/>
-      <c r="O34" s="28"/>
-      <c r="P34" s="28"/>
-      <c r="Q34" s="28"/>
-      <c r="R34" s="28"/>
-      <c r="S34" s="28"/>
-      <c r="T34" s="28"/>
-      <c r="U34" s="28"/>
-      <c r="V34" s="28"/>
-      <c r="W34" s="28"/>
+      <c r="A34" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="29"/>
+      <c r="R34" s="29"/>
+      <c r="S34" s="29"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="29"/>
+      <c r="V34" s="29"/>
+      <c r="W34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="29"/>
+      <c r="A35" s="30"/>
       <c r="W35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
       <c r="I36" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -1588,22 +1693,22 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
       <c r="W37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
       <c r="W38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,30 +1716,31 @@
       <c r="W39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="24"/>
-      <c r="O40" s="24"/>
-      <c r="P40" s="24"/>
-      <c r="Q40" s="24"/>
-      <c r="R40" s="24"/>
-      <c r="S40" s="24"/>
-      <c r="T40" s="24"/>
-      <c r="U40" s="24"/>
-      <c r="V40" s="24"/>
-      <c r="W40" s="25"/>
-    </row>
+      <c r="A40" s="24"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="25"/>
+      <c r="S40" s="25"/>
+      <c r="T40" s="25"/>
+      <c r="U40" s="25"/>
+      <c r="V40" s="25"/>
+      <c r="W40" s="26"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="35">
     <mergeCell ref="A1:R1"/>
@@ -1658,8 +1764,8 @@
     <mergeCell ref="R12:U12"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="R13:U13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="A15:W15"/>
+    <mergeCell ref="A14:W14"/>
+    <mergeCell ref="A15:W18"/>
     <mergeCell ref="I20:N20"/>
     <mergeCell ref="I21:N23"/>
     <mergeCell ref="A28:W28"/>
@@ -1725,7 +1831,7 @@
       <c r="R1" s="2"/>
       <c r="S1" s="3"/>
       <c r="T1" s="4" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
@@ -1738,7 +1844,7 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1764,7 +1870,7 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1791,9 +1897,9 @@
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1801,7 +1907,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -1820,9 +1926,9 @@
       <c r="V5" s="8"/>
       <c r="W5" s="9"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1830,7 +1936,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -1849,7 +1955,7 @@
       <c r="V6" s="8"/>
       <c r="W6" s="9"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1860,7 +1966,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="10" t="n">
         <f aca="true">TODAY()</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -1869,7 +1975,7 @@
         <v>7</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
@@ -1881,7 +1987,7 @@
       <c r="V7" s="12"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1914,7 +2020,7 @@
       </c>
       <c r="F9" s="10" t="n">
         <f aca="true">TODAY()</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -1939,7 +2045,7 @@
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
       <c r="P10" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
@@ -1954,7 +2060,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
@@ -1977,16 +2083,16 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
@@ -1994,7 +2100,7 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
@@ -2003,16 +2109,16 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="L13" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
@@ -2020,7 +2126,7 @@
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
@@ -2029,16 +2135,16 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="15" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
@@ -2055,10 +2161,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
@@ -2076,9 +2182,9 @@
       <c r="V15" s="15"/>
       <c r="W15" s="9"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -2105,19 +2211,19 @@
     </row>
     <row r="17" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="W17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="16.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="W18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="W19" s="9"/>
     </row>
@@ -2128,7 +2234,7 @@
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13"/>
       <c r="I21" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2139,83 +2245,83 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
       <c r="W22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
       <c r="W23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
       <c r="W24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="25"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="25"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
@@ -2225,7 +2331,7 @@
       <c r="A28" s="5"/>
       <c r="W28" s="9"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
         <v>3</v>
       </c>
@@ -2252,9 +2358,9 @@
       <c r="V29" s="7"/>
       <c r="W29" s="7"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -2282,9 +2388,9 @@
       <c r="V30" s="8"/>
       <c r="W30" s="9"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -2312,7 +2418,7 @@
       <c r="V31" s="8"/>
       <c r="W31" s="9"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
         <v>6</v>
       </c>
@@ -2323,7 +2429,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="10" t="n">
         <f aca="false">G7</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
@@ -2331,18 +2437,18 @@
       <c r="L32" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="N32" s="26" t="str">
+      <c r="N32" s="27" t="str">
         <f aca="false">N7</f>
         <v>PROMOTOR</v>
       </c>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
-      <c r="Q32" s="26"/>
-      <c r="R32" s="26"/>
-      <c r="S32" s="26"/>
-      <c r="T32" s="26"/>
-      <c r="U32" s="26"/>
-      <c r="V32" s="26"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="27"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="27"/>
+      <c r="U32" s="27"/>
+      <c r="V32" s="27"/>
       <c r="W32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,7 +2461,7 @@
       </c>
       <c r="F34" s="10" t="n">
         <f aca="false">F9</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -2363,45 +2469,45 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
-      <c r="H35" s="27"/>
-      <c r="S35" s="27"/>
+      <c r="H35" s="28"/>
+      <c r="S35" s="28"/>
       <c r="W35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
-      <c r="N36" s="28"/>
-      <c r="O36" s="28"/>
-      <c r="P36" s="28"/>
-      <c r="Q36" s="28"/>
-      <c r="R36" s="28"/>
-      <c r="S36" s="28"/>
-      <c r="T36" s="28"/>
-      <c r="U36" s="28"/>
-      <c r="V36" s="28"/>
-      <c r="W36" s="28"/>
+      <c r="A36" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="29"/>
+      <c r="S36" s="29"/>
+      <c r="T36" s="29"/>
+      <c r="U36" s="29"/>
+      <c r="V36" s="29"/>
+      <c r="W36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29"/>
+      <c r="A37" s="30"/>
       <c r="W37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
       <c r="I38" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -2412,22 +2518,22 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
       <c r="W39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
       <c r="W40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2435,29 +2541,29 @@
       <c r="W41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="24"/>
-      <c r="O42" s="24"/>
-      <c r="P42" s="24"/>
-      <c r="Q42" s="24"/>
-      <c r="R42" s="24"/>
-      <c r="S42" s="24"/>
-      <c r="T42" s="24"/>
-      <c r="U42" s="24"/>
-      <c r="V42" s="24"/>
-      <c r="W42" s="25"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="25"/>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="25"/>
+      <c r="S42" s="25"/>
+      <c r="T42" s="25"/>
+      <c r="U42" s="25"/>
+      <c r="V42" s="25"/>
+      <c r="W42" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -2553,7 +2659,7 @@
       <c r="R1" s="2"/>
       <c r="S1" s="3"/>
       <c r="T1" s="4" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
@@ -2566,7 +2672,7 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -2592,7 +2698,7 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2619,9 +2725,9 @@
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2629,7 +2735,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2648,9 +2754,9 @@
       <c r="V5" s="8"/>
       <c r="W5" s="9"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2658,7 +2764,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2677,7 +2783,7 @@
       <c r="V6" s="8"/>
       <c r="W6" s="9"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -2688,7 +2794,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="10" t="n">
         <f aca="true">TODAY()</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -2697,7 +2803,7 @@
         <v>7</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
@@ -2709,7 +2815,7 @@
       <c r="V7" s="12"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -2742,7 +2848,7 @@
       </c>
       <c r="F9" s="10" t="n">
         <f aca="true">TODAY()</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -2767,7 +2873,7 @@
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
       <c r="P10" s="16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
@@ -2782,7 +2888,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
@@ -2805,16 +2911,16 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
@@ -2822,7 +2928,7 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
@@ -2831,16 +2937,16 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="L13" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
@@ -2848,7 +2954,7 @@
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
@@ -2857,16 +2963,16 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="15" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
@@ -2883,10 +2989,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
@@ -2904,9 +3010,9 @@
       <c r="V15" s="15"/>
       <c r="W15" s="9"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -2933,19 +3039,19 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="W17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="W18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="W19" s="9"/>
     </row>
@@ -2956,7 +3062,7 @@
     <row r="21" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13"/>
       <c r="I21" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2967,83 +3073,83 @@
     </row>
     <row r="22" customFormat="false" ht="16.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="13"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
       <c r="W22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
       <c r="W23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
       <c r="W24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="25"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="25"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
@@ -3053,7 +3159,7 @@
       <c r="A28" s="5"/>
       <c r="W28" s="9"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
         <v>3</v>
       </c>
@@ -3080,9 +3186,9 @@
       <c r="V29" s="7"/>
       <c r="W29" s="7"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -3110,9 +3216,9 @@
       <c r="V30" s="8"/>
       <c r="W30" s="9"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -3140,7 +3246,7 @@
       <c r="V31" s="8"/>
       <c r="W31" s="9"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
         <v>6</v>
       </c>
@@ -3151,7 +3257,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="10" t="n">
         <f aca="false">G7</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
@@ -3159,18 +3265,18 @@
       <c r="L32" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="N32" s="26" t="str">
+      <c r="N32" s="27" t="str">
         <f aca="false">N7</f>
         <v>Ejecutivo comercial</v>
       </c>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
-      <c r="Q32" s="26"/>
-      <c r="R32" s="26"/>
-      <c r="S32" s="26"/>
-      <c r="T32" s="26"/>
-      <c r="U32" s="26"/>
-      <c r="V32" s="26"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="27"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="27"/>
+      <c r="U32" s="27"/>
+      <c r="V32" s="27"/>
       <c r="W32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3183,7 +3289,7 @@
       </c>
       <c r="F34" s="10" t="n">
         <f aca="false">F9</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -3191,45 +3297,45 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
-      <c r="H35" s="27"/>
-      <c r="S35" s="27"/>
+      <c r="H35" s="28"/>
+      <c r="S35" s="28"/>
       <c r="W35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
-      <c r="N36" s="28"/>
-      <c r="O36" s="28"/>
-      <c r="P36" s="28"/>
-      <c r="Q36" s="28"/>
-      <c r="R36" s="28"/>
-      <c r="S36" s="28"/>
-      <c r="T36" s="28"/>
-      <c r="U36" s="28"/>
-      <c r="V36" s="28"/>
-      <c r="W36" s="28"/>
+      <c r="A36" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="29"/>
+      <c r="S36" s="29"/>
+      <c r="T36" s="29"/>
+      <c r="U36" s="29"/>
+      <c r="V36" s="29"/>
+      <c r="W36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29"/>
+      <c r="A37" s="30"/>
       <c r="W37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
       <c r="I38" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -3240,22 +3346,22 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
       <c r="W39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
       <c r="W40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,29 +3369,29 @@
       <c r="W41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="24"/>
-      <c r="O42" s="24"/>
-      <c r="P42" s="24"/>
-      <c r="Q42" s="24"/>
-      <c r="R42" s="24"/>
-      <c r="S42" s="24"/>
-      <c r="T42" s="24"/>
-      <c r="U42" s="24"/>
-      <c r="V42" s="24"/>
-      <c r="W42" s="25"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="25"/>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="25"/>
+      <c r="S42" s="25"/>
+      <c r="T42" s="25"/>
+      <c r="U42" s="25"/>
+      <c r="V42" s="25"/>
+      <c r="W42" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="39">

</xml_diff>

<commit_message>
Cambio de la aplicacion los cargos son ahora una tabla de la BD
</commit_message>
<xml_diff>
--- a/AdministradorTI/archivos/plantillas_excel/PLANTILLA-USUARIOS-NUEVOS.xlsx
+++ b/AdministradorTI/archivos/plantillas_excel/PLANTILLA-USUARIOS-NUEVOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEONARD\python-dev\incasur-projecto\AdministradorTI\archivos\plantillas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01604D7-0CB2-4B04-ABF1-748AB8DDA4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C8E372-9466-43A3-95A3-5EE875F8F978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>CRAC INCASUR S.A.</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Usuario SBS:</t>
-  </si>
-  <si>
-    <t>bcarpioa</t>
   </si>
   <si>
     <t>Usuario Impresora:</t>
@@ -498,7 +495,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -513,36 +510,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -551,23 +547,30 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -787,7 +790,7 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI11" sqref="AI11"/>
+      <selection activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.3984375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -798,446 +801,447 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
       <c r="S1" s="1"/>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
     </row>
     <row r="2" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
     </row>
     <row r="3" spans="1:23" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
     </row>
     <row r="4" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
     </row>
     <row r="5" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="10" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
       <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="18">
         <f ca="1">TODAY()</f>
         <v>46052</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
       <c r="L6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
       <c r="W6" s="3"/>
     </row>
     <row r="7" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
     </row>
     <row r="8" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="18">
         <f ca="1">TODAY()</f>
         <v>46052</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
       <c r="W8" s="3"/>
     </row>
     <row r="9" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
       <c r="L9" t="s">
         <v>13</v>
       </c>
-      <c r="P9" s="22" t="s">
+      <c r="P9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
     </row>
     <row r="10" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
       <c r="L10" t="s">
         <v>17</v>
       </c>
-      <c r="R10" s="23" t="s">
+      <c r="R10" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+    <row r="11" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="27" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="10" t="s">
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="28"/>
-    </row>
-    <row r="12" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="11"/>
+    </row>
+    <row r="12" spans="1:23" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
       <c r="L12" t="s">
         <v>24</v>
       </c>
-      <c r="R12" s="18" t="s">
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="W12" s="3"/>
+    </row>
+    <row r="13" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="W12" s="3"/>
-    </row>
-    <row r="13" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="H13" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" t="s">
+      <c r="M13" s="10"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="31"/>
+    </row>
+    <row r="14" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="R13" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="W13" s="3"/>
-    </row>
-    <row r="14" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+    </row>
+    <row r="15" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="20"/>
-      <c r="W14" s="20"/>
-    </row>
-    <row r="15" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+    </row>
+    <row r="16" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-    </row>
-    <row r="16" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+    </row>
+    <row r="17" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-    </row>
-    <row r="17" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
     </row>
     <row r="18" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
     </row>
     <row r="19" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -1245,44 +1249,44 @@
     </row>
     <row r="20" spans="1:23" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="I20" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
+      <c r="I20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
       <c r="W20" s="3"/>
     </row>
     <row r="21" spans="1:23" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
       <c r="W21" s="3"/>
     </row>
     <row r="22" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
       <c r="W22" s="3"/>
     </row>
     <row r="23" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
       <c r="W23" s="3"/>
     </row>
     <row r="24" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
@@ -1344,93 +1348,93 @@
       <c r="W27" s="3"/>
     </row>
     <row r="28" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-      <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
-      <c r="U28" s="12"/>
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="16"/>
     </row>
     <row r="29" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="10" t="str">
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17" t="str">
         <f>G5</f>
         <v>CARPIO ARAGON</v>
       </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="10"/>
-      <c r="V29" s="10"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
       <c r="W29" s="3"/>
     </row>
     <row r="30" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="13">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="18">
         <f ca="1">G6</f>
         <v>46052</v>
       </c>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
       <c r="L30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N30" s="24" t="str">
+      <c r="N30" s="19" t="str">
         <f>N6</f>
         <v>EJECUTIVO COMERCIAL</v>
       </c>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
       <c r="W30" s="3"/>
     </row>
     <row r="31" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
@@ -1441,12 +1445,12 @@
       <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="18">
         <f ca="1">F8</f>
         <v>46052</v>
       </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="W32" s="3"/>
     </row>
     <row r="33" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
@@ -1456,31 +1460,31 @@
       <c r="W33" s="3"/>
     </row>
     <row r="34" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="14"/>
-      <c r="V34" s="14"/>
-      <c r="W34" s="14"/>
+      <c r="A34" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="29"/>
+      <c r="R34" s="29"/>
+      <c r="S34" s="29"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="29"/>
+      <c r="V34" s="29"/>
+      <c r="W34" s="29"/>
     </row>
     <row r="35" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
@@ -1488,34 +1492,34 @@
     </row>
     <row r="36" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="I36" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
+      <c r="I36" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
       <c r="W36" s="3"/>
     </row>
     <row r="37" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
+      <c r="N37" s="28"/>
       <c r="W37" s="3"/>
     </row>
     <row r="38" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
       <c r="W38" s="3"/>
     </row>
     <row r="39" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
@@ -1550,34 +1554,6 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="T1:W3"/>
-    <mergeCell ref="A3:R3"/>
-    <mergeCell ref="A4:W4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="G5:V5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="N6:V6"/>
-    <mergeCell ref="A7:W7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:K9"/>
-    <mergeCell ref="P9:W9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="R10:U10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="R11:U11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="R12:U12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="R13:U13"/>
-    <mergeCell ref="A14:W14"/>
-    <mergeCell ref="A15:W18"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="I21:N23"/>
-    <mergeCell ref="A28:W28"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="G29:V29"/>
     <mergeCell ref="I36:N36"/>
     <mergeCell ref="I37:N38"/>
     <mergeCell ref="A30:F30"/>
@@ -1585,6 +1561,34 @@
     <mergeCell ref="N30:V30"/>
     <mergeCell ref="F32:H32"/>
     <mergeCell ref="A34:W34"/>
+    <mergeCell ref="A15:W18"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I21:N23"/>
+    <mergeCell ref="A28:W28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="G29:V29"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="R12:U12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A14:W14"/>
+    <mergeCell ref="O13:W13"/>
+    <mergeCell ref="F9:K9"/>
+    <mergeCell ref="P9:W9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="R10:U10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="R11:U11"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="N6:V6"/>
+    <mergeCell ref="A7:W7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="T1:W3"/>
+    <mergeCell ref="A3:R3"/>
+    <mergeCell ref="A4:W4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="G5:V5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>